<commit_message>
new module, create excel and summary migration
</commit_message>
<xml_diff>
--- a/Output/excel_output/stp_mst_status_20250904_183017.xlsx
+++ b/Output/excel_output/stp_mst_status_20250904_183017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanNava\PycharmProjects\PythonProject\Optus_Topology_Creator\Output\excel_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9821DEC-1CA0-4C13-B07C-804D7471E841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F5EB18-8280-465A-A4EF-3C6DCF65DEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -929,7 +929,7 @@
   <dimension ref="A1:I476"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F297" sqref="F297"/>
+      <selection activeCell="D27" sqref="D27:D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>